<commit_message>
move simpleton data to settings simpleton tab
</commit_message>
<xml_diff>
--- a/testdata/settings.example.xlsx
+++ b/testdata/settings.example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC81CBFC-978C-5540-8B69-2B1923B602FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC21C9CD-3256-084A-990B-B87EFBAA098E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-24840" windowWidth="21600" windowHeight="37940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>url</t>
   </si>
@@ -113,9 +113,6 @@
     <t>selectorNum</t>
   </si>
   <si>
-    <t>tabName</t>
-  </si>
-  <si>
     <t>t2cu</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>ARCONICTP_HJBB 06.15.2020</t>
   </si>
   <si>
-    <t>simpletonTest</t>
-  </si>
-  <si>
     <t>ARCONIC</t>
   </si>
   <si>
@@ -155,13 +149,40 @@
     <t>ARCONIC_HJBTnewsorting 6.15.20</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
     <t>JISQHX3</t>
   </si>
   <si>
     <t>https://order-tst-prof2.nonprod.jbhunt.com/order/automationrules</t>
+  </si>
+  <si>
+    <t>Trading Partner</t>
+  </si>
+  <si>
+    <t>SCAC</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>Corp Acct</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>Fleet</t>
+  </si>
+  <si>
+    <t>ALPI37</t>
+  </si>
+  <si>
+    <t>ICS</t>
+  </si>
+  <si>
+    <t>Brok</t>
   </si>
 </sst>
 </file>
@@ -333,7 +354,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,6 +537,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,15 +778,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -768,6 +793,11 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="42" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -814,7 +844,202 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="64">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1267,130 +1492,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2298,7 +2399,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9BB73794-A3F9-7840-AB43-105336261E1A}" name="Table79" displayName="Table79" ref="A1:D3" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9BB73794-A3F9-7840-AB43-105336261E1A}" name="Table79" displayName="Table79" ref="A1:D3" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="A1:D3" xr:uid="{D902FDEF-4A66-A249-8A9E-4C9476CD0585}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2306,17 +2407,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{40FB39B6-E6C9-E04C-8DC5-7B1EF7CF03CD}" name="url" dataDxfId="53" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{5E56D9C9-F570-1348-8269-D0AD78470E72}" name="delaySecond" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{3FE4A58A-3B03-0F45-9086-BD7CC36ED774}" name="username" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{75FC3F85-123C-734E-A443-F78AC8D89B27}" name="password" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{40FB39B6-E6C9-E04C-8DC5-7B1EF7CF03CD}" name="url" dataDxfId="58" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{5E56D9C9-F570-1348-8269-D0AD78470E72}" name="delaySecond" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{3FE4A58A-3B03-0F45-9086-BD7CC36ED774}" name="username" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{75FC3F85-123C-734E-A443-F78AC8D89B27}" name="password" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:D3" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:D3" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
   <autoFilter ref="A1:D3" xr:uid="{53489C08-B6AB-264E-AD35-1FF7F63D170E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2324,17 +2425,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{9F00E9D8-F9CB-714B-8445-E26440DB3957}" name="tradingPartner" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{50F81C84-FE38-A44D-A41E-61752D4C3DC4}" name="createdBy" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{043C2551-D34E-364E-8939-D3F2091FAD79}" name="selectorTotal" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{8F70CAE4-FFF8-DC45-9394-34D962370E61}" name="selectorNum" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{9F00E9D8-F9CB-714B-8445-E26440DB3957}" name="tradingPartner" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{50F81C84-FE38-A44D-A41E-61752D4C3DC4}" name="createdBy" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{043C2551-D34E-364E-8939-D3F2091FAD79}" name="selectorTotal" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{8F70CAE4-FFF8-DC45-9394-34D962370E61}" name="selectorNum" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:L3" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:L3" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="A1:L3" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2350,39 +2451,49 @@
     <filterColumn colId="11" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A02382E6-ADE3-A242-A202-192BBD90FAE7}" name="tradingPartner" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{74C6A343-DC32-3F4A-853C-100B3FC0E934}" name="fileName" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{A9E05B2F-FEED-424F-A6A7-6CB274608CBD}" name="t1bt" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{1872C4F0-C20C-AA44-8D7F-0C51AAC58F25}" name="t2bt" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{A576BB00-6B6F-AC42-8642-6CF7825FCABD}" name="t1bu" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{579AEECD-3CAD-794A-8DD3-324A8BD3E83C}" name="t2bu" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{75E0BC80-D6B0-C848-B965-EB9E71ED84FA}" name="t1so" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{D8392679-15A0-EA4D-A15D-8C3DD767BA31}" name="t2so" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{E46D819F-6CE5-1443-BC5D-6679813EE74A}" name="t1fl" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{BFD61505-7B07-6D48-8F42-187515D288C2}" name="t2fl" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{34C9D25B-DA7B-A745-9F3C-CD55679D0E9A}" name="t1cu" dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{0AEE78C2-385D-6948-A98E-236D5ECBC3FF}" name="t2cu" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{A02382E6-ADE3-A242-A202-192BBD90FAE7}" name="tradingPartner" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{74C6A343-DC32-3F4A-853C-100B3FC0E934}" name="fileName" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{A9E05B2F-FEED-424F-A6A7-6CB274608CBD}" name="t1bt" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{1872C4F0-C20C-AA44-8D7F-0C51AAC58F25}" name="t2bt" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{A576BB00-6B6F-AC42-8642-6CF7825FCABD}" name="t1bu" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{579AEECD-3CAD-794A-8DD3-324A8BD3E83C}" name="t2bu" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{75E0BC80-D6B0-C848-B965-EB9E71ED84FA}" name="t1so" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{D8392679-15A0-EA4D-A15D-8C3DD767BA31}" name="t2so" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{E46D819F-6CE5-1443-BC5D-6679813EE74A}" name="t1fl" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{BFD61505-7B07-6D48-8F42-187515D288C2}" name="t2fl" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{34C9D25B-DA7B-A745-9F3C-CD55679D0E9A}" name="t1cu" dataDxfId="30"/>
+    <tableColumn id="12" xr3:uid="{0AEE78C2-385D-6948-A98E-236D5ECBC3FF}" name="t2cu" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:B2" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:B2" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{21176821-3178-9C43-9AC9-BD166EC5CBF1}" name="Table102" displayName="Table102" ref="A1:G3" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:G3" xr:uid="{ABD8C002-5C91-5547-833F-9725E98EC1BA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{85030897-D1E7-2C43-974D-6C721A342EBB}" name="fileName" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{BBEC5B11-0741-8D44-8E5D-01804D7A4C02}" name="tabName" dataDxfId="18"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{5549F14E-FA76-794E-917B-DBF23F817732}" name="Trading Partner" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{0517727C-97CD-D248-AA59-A807DC9E0DA5}" name="SCAC" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{0407C1B6-E411-CF44-A5E6-0B9E3547CA68}" name="BTC" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{A3FD7055-58B1-2C4B-AE88-5DAA620ACC68}" name="Corp Acct" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{F4FE6365-5C74-D842-89E7-5D327D28E377}" name="BU" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{3577535F-9D1A-E647-87D2-94D0A82ED9BF}" name="SO" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{30D526E9-7996-3844-A461-C59C339F7969}" name="Fleet" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5FBCBAA8-0386-4B4F-8826-46FD915F103C}" name="Table11" displayName="Table11" ref="A1:M2" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5FBCBAA8-0386-4B4F-8826-46FD915F103C}" name="Table11" displayName="Table11" ref="A1:M2" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="A1:M2" xr:uid="{B5B17CF2-012E-764F-A3B1-44C7505ECF30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2399,19 +2510,19 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D5F5E6A1-2B72-7F41-8016-996CDA62DE12}" name="missingCodeFileName" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{741294D1-F604-CC4A-917D-9BFEC40EA974}" name="ruleDataFileName" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{D90BCCCC-60DE-E140-8EA8-9C68920FC3E3}" name="newFileName" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{0F1C21AD-5DCA-2445-AAD5-65278C3DA304}" name="t1bt" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{831B61E6-9836-7E43-AD5B-689EC75DC91F}" name="t2bt" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{967D2A40-3B01-A44A-8EC4-DE08B2A7DB9C}" name="t1bu" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{1F9B7FB5-ED4F-F049-9579-548D513A89A5}" name="t2bu" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{3894DDE8-0A5C-C346-BE15-6A8842257ABE}" name="t1so" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{488C3AE5-D292-EE4C-AAB0-F85A3C34E5BB}" name="t2so" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{5E123C06-E039-CB4F-886C-B626069D549C}" name="t1fl" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{3B39AD1D-E4D3-B54A-86CE-68BC61D6D409}" name="t2fl" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{724A8853-215F-E941-B4A2-B96EC61D4648}" name="t1cu" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{908C0810-E77F-474C-8C5D-79C69A3CE84C}" name="t2cu" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D5F5E6A1-2B72-7F41-8016-996CDA62DE12}" name="missingCodeFileName" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{741294D1-F604-CC4A-917D-9BFEC40EA974}" name="ruleDataFileName" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{D90BCCCC-60DE-E140-8EA8-9C68920FC3E3}" name="newFileName" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{0F1C21AD-5DCA-2445-AAD5-65278C3DA304}" name="t1bt" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{831B61E6-9836-7E43-AD5B-689EC75DC91F}" name="t2bt" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{967D2A40-3B01-A44A-8EC4-DE08B2A7DB9C}" name="t1bu" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{1F9B7FB5-ED4F-F049-9579-548D513A89A5}" name="t2bu" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{3894DDE8-0A5C-C346-BE15-6A8842257ABE}" name="t1so" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{488C3AE5-D292-EE4C-AAB0-F85A3C34E5BB}" name="t2so" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{5E123C06-E039-CB4F-886C-B626069D549C}" name="t1fl" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{3B39AD1D-E4D3-B54A-86CE-68BC61D6D409}" name="t2fl" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{724A8853-215F-E941-B4A2-B96EC61D4648}" name="t1cu" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{908C0810-E77F-474C-8C5D-79C69A3CE84C}" name="t2cu" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2716,7 +2827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9160359D-1B9E-284A-A763-80B627CB8CD3}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2730,22 +2841,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>34</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>45</v>
+      <c r="A2" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
@@ -2754,7 +2865,7 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
@@ -2788,22 +2899,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -2815,10 +2926,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
@@ -2852,49 +2963,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="K1" s="7" t="s">
         <v>30</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>9</v>
@@ -2921,18 +3032,18 @@
         <v>15</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
@@ -2959,18 +3070,18 @@
         <v>15</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>9</v>
@@ -2997,18 +3108,18 @@
         <v>15</v>
       </c>
       <c r="K4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
@@ -3035,10 +3146,10 @@
         <v>15</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3051,53 +3162,87 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F814824A-BE6E-4AC5-90CF-CA8866E1DFA9}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="A1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="A2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3123,44 +3268,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>30</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">

</xml_diff>